<commit_message>
changed python code to pep8 style
</commit_message>
<xml_diff>
--- a/tools/test-data/mutant_reads_summary_short_trim_test_data_VA.xlsx
+++ b/tools/test-data/mutant_reads_summary_short_trim_test_data_VA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="186">
   <si>
     <t>tag</t>
   </si>
@@ -123,201 +123,426 @@
     <t>variant ID</t>
   </si>
   <si>
+    <t>GATAACCTTGCTTCGTGATTAATC</t>
+  </si>
+  <si>
+    <t>ab1.ba2</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions</t>
+  </si>
+  <si>
+    <t>505</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions-505-C-A</t>
+  </si>
+  <si>
+    <t>ab2.ba1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>GATTGGATAACGTTGTGGCAATTG</t>
   </si>
   <si>
-    <t>ab1.ba2</t>
-  </si>
-  <si>
-    <t>ACH_TDII_5regions</t>
-  </si>
-  <si>
-    <t>505</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>571</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions-571-C-T</t>
+  </si>
+  <si>
+    <t>CCTCCCGGCAGTGCGAAAATGTCA</t>
+  </si>
+  <si>
+    <t>958</t>
+  </si>
+  <si>
+    <t>ACH_TDII_5regions-958-T-C</t>
+  </si>
+  <si>
+    <t>cvrg (Du Novo)</t>
+  </si>
+  <si>
+    <t>tier 1.1</t>
+  </si>
+  <si>
+    <t>AF 1.1</t>
+  </si>
+  <si>
+    <t>tier 1.2</t>
+  </si>
+  <si>
+    <t>AF 1.2</t>
+  </si>
+  <si>
+    <t>tier 2.1</t>
+  </si>
+  <si>
+    <t>AF 2.1</t>
+  </si>
+  <si>
+    <t>tier 2.2</t>
+  </si>
+  <si>
+    <t>AF 2.2</t>
+  </si>
+  <si>
+    <t>tier 2.3</t>
+  </si>
+  <si>
+    <t>AF 2.3</t>
+  </si>
+  <si>
+    <t>tier 2.4</t>
+  </si>
+  <si>
+    <t>AF 2.4</t>
+  </si>
+  <si>
+    <t>tier 3.1</t>
+  </si>
+  <si>
+    <t>AF 3.1</t>
+  </si>
+  <si>
+    <t>tier 4</t>
+  </si>
+  <si>
+    <t>AF 4</t>
+  </si>
+  <si>
+    <t>AF 1.1-1.2</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.1</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.2</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.3</t>
+  </si>
+  <si>
+    <t>AF 1.1-2.4</t>
+  </si>
+  <si>
+    <t>AF 1.1-3.1</t>
+  </si>
+  <si>
+    <t>AF 1.1-4</t>
+  </si>
+  <si>
+    <t>cvrg (VA)</t>
+  </si>
+  <si>
+    <t>tier count</t>
+  </si>
+  <si>
+    <t>AF (VA)</t>
+  </si>
+  <si>
+    <t>alt. allele (Du Novo)</t>
+  </si>
+  <si>
+    <t>AF (Du Novo)</t>
+  </si>
+  <si>
+    <t>ref. allele (Du Novo)</t>
+  </si>
+  <si>
+    <t>tier</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Description of tiers with examples</t>
+  </si>
+  <si>
+    <t>Tier 1.1</t>
+  </si>
+  <si>
+    <t>both ab and ba SSCS present (&gt;75% of the sites with alternative base) and minimal FS&gt;=3 for both SSCS in at least one mate</t>
+  </si>
+  <si>
+    <t>AAAAAGATGCCGACTACCTT</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000</t>
+  </si>
+  <si>
+    <t>11068</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4081</t>
+  </si>
+  <si>
+    <t>4098</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000-11068-C-G</t>
+  </si>
+  <si>
+    <t>AAAAATGCGTAGAAATATGC</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Tier 1.2</t>
+  </si>
+  <si>
+    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and mate pair validation (min. FS=1) and minimal FS&gt;=3 for at least one of the SSCS</t>
+  </si>
+  <si>
+    <t>CTATGACCCGTGAGCCCATG</t>
+  </si>
+  <si>
+    <t>10776</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>47170</t>
+  </si>
+  <si>
+    <t>41149</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000-10776-G-T</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Tier 2.1</t>
+  </si>
+  <si>
+    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and minimal FS&gt;=3 for at least one of the SSCS in at least one mate</t>
+  </si>
+  <si>
+    <t>AAAAAAACATCATACACCCA</t>
+  </si>
+  <si>
+    <t>246</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>2.1</t>
   </si>
   <si>
-    <t>ACH_TDII_5regions-505-C-A</t>
-  </si>
-  <si>
-    <t>ab2.ba1</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>571</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>ACH_TDII_5regions-571-C-T</t>
-  </si>
-  <si>
-    <t>CCTCCCGGCAGTGCGAAAATGTCA</t>
-  </si>
-  <si>
-    <t>958</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>ACH_TDII_5regions-958-T-C</t>
-  </si>
-  <si>
-    <t>cvrg (Du Novo)</t>
-  </si>
-  <si>
-    <t>tier 1.1</t>
-  </si>
-  <si>
-    <t>AF 1.1</t>
-  </si>
-  <si>
-    <t>tier 1.2</t>
-  </si>
-  <si>
-    <t>AF 1.2</t>
-  </si>
-  <si>
-    <t>tier 2.1</t>
-  </si>
-  <si>
-    <t>AF 2.1</t>
-  </si>
-  <si>
-    <t>tier 2.2</t>
-  </si>
-  <si>
-    <t>AF 2.2</t>
-  </si>
-  <si>
-    <t>tier 2.3</t>
-  </si>
-  <si>
-    <t>AF 2.3</t>
-  </si>
-  <si>
-    <t>tier 2.4</t>
-  </si>
-  <si>
-    <t>AF 2.4</t>
-  </si>
-  <si>
-    <t>tier 3.1</t>
-  </si>
-  <si>
-    <t>AF 3.1</t>
-  </si>
-  <si>
-    <t>tier 4</t>
-  </si>
-  <si>
-    <t>AF 4</t>
-  </si>
-  <si>
-    <t>AF 1.1-1.2</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.1</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.2</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.3</t>
-  </si>
-  <si>
-    <t>AF 1.1-2.4</t>
-  </si>
-  <si>
-    <t>AF 1.1-3.1</t>
-  </si>
-  <si>
-    <t>AF 1.1-4</t>
-  </si>
-  <si>
-    <t>cvrg (VA)</t>
-  </si>
-  <si>
-    <t>tier count</t>
-  </si>
-  <si>
-    <t>AF (VA)</t>
-  </si>
-  <si>
-    <t>alt. allele (Du Novo)</t>
-  </si>
-  <si>
-    <t>AF (Du Novo)</t>
-  </si>
-  <si>
-    <t>ref. allele (Du Novo)</t>
-  </si>
-  <si>
-    <t>tier</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>Description of tiers with examples</t>
-  </si>
-  <si>
-    <t>Tier 1.1</t>
-  </si>
-  <si>
-    <t>both ab and ba SSCS present (&gt;75% of the sites with alternative base) and minimal FS&gt;=3 for both SSCS in at least one mate</t>
-  </si>
-  <si>
-    <t>Tier 1.2</t>
-  </si>
-  <si>
-    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and mate pair validation (min. FS=1) and minimal FS&gt;=3 for at least one of the SSCS</t>
-  </si>
-  <si>
-    <t>Tier 2.1</t>
-  </si>
-  <si>
-    <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and minimal FS&gt;=3 for at least one of the SSCS in at least one mate</t>
-  </si>
-  <si>
     <t>Tier 2.2</t>
   </si>
   <si>
     <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and mate pair validation (min. FS=1)</t>
   </si>
   <si>
+    <t>ATCAGCCATGGCTATTATTG</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
     <t>Tier 2.3</t>
   </si>
   <si>
     <t>both ab and ba SSCS present (&gt;75% of the sites with alt. base) and minimal FS=1 for both SSCS in one mate and minimal FS&gt;=3 for at least one of the SSCS in the other mate</t>
   </si>
   <si>
+    <t>ATCAATATGGCCTCGCCACG</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
     <t>Tier 2.4</t>
   </si>
   <si>
     <t>both ab and ba SSCS present (&gt;50% of the sites with alt. base) and recurring mutation on this position</t>
   </si>
   <si>
+    <t>ATGCCTACCTCATTTGTCGT</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
     <t>Tier 3.1</t>
   </si>
   <si>
     <t>both ab and ba SSCS present (&gt;50% of the sites with alt. base) and minimal FS&gt;=1 for both SSCS in at least one mate</t>
   </si>
   <si>
+    <t>ACAACATCACGTATTCAGGT</t>
+  </si>
+  <si>
+    <t>11315</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
+  <si>
+    <t>0.333333333333333</t>
+  </si>
+  <si>
+    <t>0.666666666666667</t>
+  </si>
+  <si>
+    <t>6584</t>
+  </si>
+  <si>
+    <t>6482</t>
+  </si>
+  <si>
+    <t>Chr5:5-20000-11315-C-T</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
     <t>Tier 4</t>
   </si>
   <si>
@@ -327,9 +552,6 @@
     <t>ATGTTGTGAATAACCCACAC</t>
   </si>
   <si>
-    <t>Chr5:5-20000</t>
-  </si>
-  <si>
     <t>13983</t>
   </si>
   <si>
@@ -339,34 +561,16 @@
     <t>186</t>
   </si>
   <si>
-    <t>255</t>
-  </si>
-  <si>
     <t>276</t>
   </si>
   <si>
     <t>269</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>5348</t>
   </si>
   <si>
     <t>5350</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>Chr5:5-20000-13983-G-C</t>
@@ -853,13 +1057,13 @@
         <v>131</v>
       </c>
       <c r="F2">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="G2">
         <v>264</v>
       </c>
       <c r="H2">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="I2">
         <v>173</v>
@@ -874,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -892,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1034,7 +1238,7 @@
     </row>
     <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -1043,16 +1247,16 @@
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5">
-        <v>128</v>
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
       </c>
       <c r="F5">
         <v>217</v>
       </c>
-      <c r="G5">
-        <v>195</v>
+      <c r="G5" t="s">
+        <v>44</v>
       </c>
       <c r="H5">
         <v>284</v>
@@ -1064,19 +1268,19 @@
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1085,19 +1289,19 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>44</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
-      <c r="V5">
-        <v>1</v>
+      <c r="V5" t="s">
+        <v>44</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1127,15 +1331,15 @@
         <v>1</v>
       </c>
       <c r="AG5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -1144,19 +1348,19 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6">
-        <v>263</v>
-      </c>
-      <c r="F6">
-        <v>263</v>
-      </c>
-      <c r="G6">
-        <v>278.5</v>
-      </c>
-      <c r="H6">
-        <v>283.5</v>
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
       </c>
       <c r="I6">
         <v>143</v>
@@ -1165,19 +1369,19 @@
         <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1186,22 +1390,22 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" t="s">
+        <v>44</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1230,7 +1434,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -1239,7 +1443,7 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -1257,7 +1461,7 @@
         <v>195</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
         <v>39</v>
@@ -1323,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="AG8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AI8" t="s">
         <v>52</v>
@@ -1331,7 +1535,7 @@
     </row>
     <row r="9" spans="1:35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
@@ -1340,7 +1544,7 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>96</v>
@@ -1358,7 +1562,7 @@
         <v>195</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K9" t="s">
         <v>39</v>
@@ -1585,35 +1789,35 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
         <v>0.5</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
       <c r="Q2">
         <v>0</v>
       </c>
@@ -1624,16 +1828,16 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <v>0.5</v>
@@ -1662,76 +1866,76 @@
     </row>
     <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>0.5</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
       <c r="S3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <v>0.5</v>
@@ -1902,7 +2106,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI27"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1921,7 +2125,7 @@
         <v>54</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -1937,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -1969,7 +2173,7 @@
         <v>66</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -1977,7 +2181,7 @@
         <v>68</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -2100,256 +2304,1824 @@
         <v>87</v>
       </c>
     </row>
+    <row r="15" spans="1:35">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" t="s">
+        <v>97</v>
+      </c>
+      <c r="O15" t="s">
+        <v>98</v>
+      </c>
+      <c r="P15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>99</v>
+      </c>
+      <c r="R15" t="s">
+        <v>97</v>
+      </c>
+      <c r="S15" t="s">
+        <v>98</v>
+      </c>
+      <c r="T15" t="s">
+        <v>99</v>
+      </c>
+      <c r="U15" t="s">
+        <v>99</v>
+      </c>
+      <c r="V15" t="s">
+        <v>100</v>
+      </c>
+      <c r="W15" t="s">
+        <v>100</v>
+      </c>
+      <c r="X15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="16" spans="1:35">
       <c r="A16" t="s">
         <v>88</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:35">
-      <c r="A17" t="s">
+      <c r="D16" t="s">
         <v>90</v>
       </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35">
-      <c r="A18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>93</v>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" t="s">
+        <v>99</v>
+      </c>
+      <c r="N16" t="s">
+        <v>99</v>
+      </c>
+      <c r="O16" t="s">
+        <v>99</v>
+      </c>
+      <c r="P16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>99</v>
+      </c>
+      <c r="R16" t="s">
+        <v>97</v>
+      </c>
+      <c r="S16" t="s">
+        <v>98</v>
+      </c>
+      <c r="T16" t="s">
+        <v>44</v>
+      </c>
+      <c r="U16" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" t="s">
+        <v>44</v>
+      </c>
+      <c r="W16" t="s">
+        <v>44</v>
+      </c>
+      <c r="X16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:35">
       <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="I19" t="s">
         <v>95</v>
+      </c>
+      <c r="J19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" t="s">
+        <v>108</v>
+      </c>
+      <c r="M19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" t="s">
+        <v>108</v>
+      </c>
+      <c r="O19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P19" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>99</v>
+      </c>
+      <c r="R19" t="s">
+        <v>108</v>
+      </c>
+      <c r="S19" t="s">
+        <v>109</v>
+      </c>
+      <c r="T19" t="s">
+        <v>99</v>
+      </c>
+      <c r="U19" t="s">
+        <v>99</v>
+      </c>
+      <c r="V19" t="s">
+        <v>100</v>
+      </c>
+      <c r="W19" t="s">
+        <v>100</v>
+      </c>
+      <c r="X19" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:35">
       <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35">
-      <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
+      <c r="L20" t="s">
+        <v>112</v>
+      </c>
+      <c r="M20" t="s">
+        <v>113</v>
+      </c>
+      <c r="N20" t="s">
+        <v>104</v>
+      </c>
+      <c r="O20" t="s">
+        <v>114</v>
+      </c>
+      <c r="P20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>99</v>
+      </c>
+      <c r="R20" t="s">
+        <v>104</v>
+      </c>
+      <c r="S20" t="s">
+        <v>114</v>
+      </c>
+      <c r="T20" t="s">
+        <v>99</v>
+      </c>
+      <c r="U20" t="s">
+        <v>99</v>
+      </c>
+      <c r="V20" t="s">
+        <v>100</v>
+      </c>
+      <c r="W20" t="s">
+        <v>100</v>
+      </c>
+      <c r="X20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:35">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="I23" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="J23" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K23" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="L23" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="M23" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="N23" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="O23" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="P23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="Q23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="R23" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="S23" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="T23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="U23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="V23" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="W23" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="X23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="Y23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="Z23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AA23" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="AB23" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="AC23" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="AD23" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="AE23" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="AG23" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="AI23" t="s">
-        <v>117</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L24" t="s">
+        <v>48</v>
+      </c>
+      <c r="M24" t="s">
+        <v>100</v>
+      </c>
+      <c r="N24" t="s">
+        <v>48</v>
+      </c>
+      <c r="O24" t="s">
+        <v>100</v>
+      </c>
+      <c r="P24" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>99</v>
+      </c>
+      <c r="R24" t="s">
+        <v>48</v>
+      </c>
+      <c r="S24" t="s">
+        <v>100</v>
+      </c>
+      <c r="T24" t="s">
+        <v>99</v>
+      </c>
+      <c r="U24" t="s">
+        <v>99</v>
+      </c>
+      <c r="V24" t="s">
+        <v>100</v>
+      </c>
+      <c r="W24" t="s">
+        <v>100</v>
+      </c>
+      <c r="X24" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35">
+      <c r="A26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:35">
       <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" t="s">
+        <v>96</v>
+      </c>
+      <c r="L27" t="s">
+        <v>134</v>
+      </c>
+      <c r="M27" t="s">
+        <v>135</v>
+      </c>
+      <c r="N27" t="s">
+        <v>134</v>
+      </c>
+      <c r="O27" t="s">
+        <v>135</v>
+      </c>
+      <c r="P27" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>99</v>
+      </c>
+      <c r="R27" t="s">
+        <v>134</v>
+      </c>
+      <c r="S27" t="s">
+        <v>135</v>
+      </c>
+      <c r="T27" t="s">
+        <v>99</v>
+      </c>
+      <c r="U27" t="s">
+        <v>99</v>
+      </c>
+      <c r="V27" t="s">
+        <v>100</v>
+      </c>
+      <c r="W27" t="s">
+        <v>100</v>
+      </c>
+      <c r="X27" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC27" t="s">
         <v>102</v>
       </c>
-      <c r="B27" t="s">
+      <c r="AD27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
         <v>43</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" t="s">
+        <v>95</v>
+      </c>
+      <c r="J28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" t="s">
+        <v>96</v>
+      </c>
+      <c r="L28" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" t="s">
+        <v>99</v>
+      </c>
+      <c r="O28" t="s">
+        <v>99</v>
+      </c>
+      <c r="P28" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>99</v>
+      </c>
+      <c r="R28" t="s">
+        <v>99</v>
+      </c>
+      <c r="S28" t="s">
+        <v>99</v>
+      </c>
+      <c r="T28" t="s">
+        <v>99</v>
+      </c>
+      <c r="U28" t="s">
+        <v>99</v>
+      </c>
+      <c r="V28" t="s">
+        <v>44</v>
+      </c>
+      <c r="W28" t="s">
+        <v>44</v>
+      </c>
+      <c r="X28" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD28" t="s">
         <v>103</v>
       </c>
-      <c r="D27" t="s">
+      <c r="AE28" t="s">
         <v>104</v>
       </c>
-      <c r="E27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" t="s">
-        <v>44</v>
-      </c>
-      <c r="I27" t="s">
-        <v>109</v>
-      </c>
-      <c r="J27" t="s">
-        <v>110</v>
-      </c>
-      <c r="K27" t="s">
+    </row>
+    <row r="30" spans="1:35">
+      <c r="A30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" t="s">
+        <v>95</v>
+      </c>
+      <c r="J31" t="s">
         <v>39</v>
       </c>
-      <c r="L27" t="s">
-        <v>111</v>
-      </c>
-      <c r="M27" t="s">
-        <v>111</v>
-      </c>
-      <c r="N27" t="s">
-        <v>111</v>
-      </c>
-      <c r="O27" t="s">
-        <v>111</v>
-      </c>
-      <c r="P27" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S27" t="s">
-        <v>111</v>
-      </c>
-      <c r="T27" t="s">
-        <v>44</v>
-      </c>
-      <c r="U27" t="s">
-        <v>44</v>
-      </c>
-      <c r="V27" t="s">
-        <v>44</v>
-      </c>
-      <c r="W27" t="s">
-        <v>44</v>
-      </c>
-      <c r="X27" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE27" t="s">
+      <c r="K31" t="s">
+        <v>96</v>
+      </c>
+      <c r="L31" t="s">
+        <v>100</v>
+      </c>
+      <c r="M31" t="s">
+        <v>100</v>
+      </c>
+      <c r="N31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>100</v>
+      </c>
+      <c r="P31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>99</v>
+      </c>
+      <c r="R31" t="s">
+        <v>100</v>
+      </c>
+      <c r="S31" t="s">
+        <v>100</v>
+      </c>
+      <c r="T31" t="s">
+        <v>99</v>
+      </c>
+      <c r="U31" t="s">
+        <v>99</v>
+      </c>
+      <c r="V31" t="s">
+        <v>100</v>
+      </c>
+      <c r="W31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35">
+      <c r="A32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" t="s">
+        <v>145</v>
+      </c>
+      <c r="I32" t="s">
+        <v>95</v>
+      </c>
+      <c r="J32" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" t="s">
+        <v>96</v>
+      </c>
+      <c r="L32" t="s">
+        <v>100</v>
+      </c>
+      <c r="M32" t="s">
+        <v>100</v>
+      </c>
+      <c r="N32" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
+        <v>100</v>
+      </c>
+      <c r="P32" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>99</v>
+      </c>
+      <c r="R32" t="s">
+        <v>100</v>
+      </c>
+      <c r="S32" t="s">
+        <v>100</v>
+      </c>
+      <c r="T32" t="s">
+        <v>99</v>
+      </c>
+      <c r="U32" t="s">
+        <v>99</v>
+      </c>
+      <c r="V32" t="s">
+        <v>100</v>
+      </c>
+      <c r="W32" t="s">
+        <v>100</v>
+      </c>
+      <c r="X32" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" t="s">
+        <v>96</v>
+      </c>
+      <c r="L35" t="s">
+        <v>99</v>
+      </c>
+      <c r="M35" t="s">
+        <v>103</v>
+      </c>
+      <c r="N35" t="s">
+        <v>99</v>
+      </c>
+      <c r="O35" t="s">
+        <v>103</v>
+      </c>
+      <c r="P35" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>99</v>
+      </c>
+      <c r="R35" t="s">
+        <v>99</v>
+      </c>
+      <c r="S35" t="s">
+        <v>103</v>
+      </c>
+      <c r="T35" t="s">
+        <v>44</v>
+      </c>
+      <c r="U35" t="s">
+        <v>44</v>
+      </c>
+      <c r="V35" t="s">
+        <v>44</v>
+      </c>
+      <c r="W35" t="s">
+        <v>100</v>
+      </c>
+      <c r="X35" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36" t="s">
+        <v>96</v>
+      </c>
+      <c r="L36" t="s">
+        <v>100</v>
+      </c>
+      <c r="M36" t="s">
+        <v>97</v>
+      </c>
+      <c r="N36" t="s">
+        <v>100</v>
+      </c>
+      <c r="O36" t="s">
+        <v>97</v>
+      </c>
+      <c r="P36" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>99</v>
+      </c>
+      <c r="R36" t="s">
+        <v>100</v>
+      </c>
+      <c r="S36" t="s">
+        <v>97</v>
+      </c>
+      <c r="T36" t="s">
+        <v>99</v>
+      </c>
+      <c r="U36" t="s">
+        <v>99</v>
+      </c>
+      <c r="V36" t="s">
+        <v>100</v>
+      </c>
+      <c r="W36" t="s">
+        <v>100</v>
+      </c>
+      <c r="X36" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA36" t="s">
         <v>115</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35">
+      <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" t="s">
+        <v>97</v>
+      </c>
+      <c r="M39" t="s">
+        <v>97</v>
+      </c>
+      <c r="N39" t="s">
+        <v>97</v>
+      </c>
+      <c r="O39" t="s">
+        <v>134</v>
+      </c>
+      <c r="P39" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R39" t="s">
+        <v>99</v>
+      </c>
+      <c r="S39" t="s">
+        <v>100</v>
+      </c>
+      <c r="T39" t="s">
+        <v>100</v>
+      </c>
+      <c r="U39" t="s">
+        <v>158</v>
+      </c>
+      <c r="V39" t="s">
+        <v>99</v>
+      </c>
+      <c r="W39" t="s">
+        <v>158</v>
+      </c>
+      <c r="X39" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35">
+      <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" t="s">
+        <v>121</v>
+      </c>
+      <c r="J40" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" t="s">
+        <v>47</v>
+      </c>
+      <c r="L40" t="s">
+        <v>99</v>
+      </c>
+      <c r="M40" t="s">
+        <v>97</v>
+      </c>
+      <c r="N40" t="s">
+        <v>99</v>
+      </c>
+      <c r="O40" t="s">
+        <v>134</v>
+      </c>
+      <c r="P40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>100</v>
+      </c>
+      <c r="R40" t="s">
+        <v>99</v>
+      </c>
+      <c r="S40" t="s">
+        <v>100</v>
+      </c>
+      <c r="T40" t="s">
+        <v>44</v>
+      </c>
+      <c r="U40" t="s">
+        <v>158</v>
+      </c>
+      <c r="V40" t="s">
+        <v>44</v>
+      </c>
+      <c r="W40" t="s">
+        <v>158</v>
+      </c>
+      <c r="X40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35">
+      <c r="A42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35">
+      <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" t="s">
+        <v>166</v>
+      </c>
+      <c r="H43" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" t="s">
+        <v>167</v>
+      </c>
+      <c r="J43" t="s">
+        <v>39</v>
+      </c>
+      <c r="K43" t="s">
+        <v>47</v>
+      </c>
+      <c r="L43" t="s">
+        <v>134</v>
+      </c>
+      <c r="M43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N43" t="s">
+        <v>134</v>
+      </c>
+      <c r="O43" t="s">
+        <v>97</v>
+      </c>
+      <c r="P43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>100</v>
+      </c>
+      <c r="R43" t="s">
+        <v>134</v>
+      </c>
+      <c r="S43" t="s">
+        <v>134</v>
+      </c>
+      <c r="T43" t="s">
+        <v>99</v>
+      </c>
+      <c r="U43" t="s">
+        <v>168</v>
+      </c>
+      <c r="V43" t="s">
+        <v>100</v>
+      </c>
+      <c r="W43" t="s">
+        <v>169</v>
+      </c>
+      <c r="X43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35">
+      <c r="A44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" t="s">
+        <v>166</v>
+      </c>
+      <c r="H44" t="s">
+        <v>174</v>
+      </c>
+      <c r="I44" t="s">
+        <v>167</v>
+      </c>
+      <c r="J44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" t="s">
+        <v>47</v>
+      </c>
+      <c r="L44" t="s">
+        <v>134</v>
+      </c>
+      <c r="M44" t="s">
+        <v>97</v>
+      </c>
+      <c r="N44" t="s">
+        <v>134</v>
+      </c>
+      <c r="O44" t="s">
+        <v>97</v>
+      </c>
+      <c r="P44" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>100</v>
+      </c>
+      <c r="R44" t="s">
+        <v>134</v>
+      </c>
+      <c r="S44" t="s">
+        <v>134</v>
+      </c>
+      <c r="T44" t="s">
+        <v>99</v>
+      </c>
+      <c r="U44" t="s">
+        <v>168</v>
+      </c>
+      <c r="V44" t="s">
+        <v>100</v>
+      </c>
+      <c r="W44" t="s">
+        <v>169</v>
+      </c>
+      <c r="X44" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35">
+      <c r="A46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35">
+      <c r="A47" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" t="s">
+        <v>179</v>
+      </c>
+      <c r="F47" t="s">
+        <v>180</v>
+      </c>
+      <c r="G47" t="s">
+        <v>151</v>
+      </c>
+      <c r="H47" t="s">
+        <v>181</v>
+      </c>
+      <c r="I47" t="s">
+        <v>182</v>
+      </c>
+      <c r="J47" t="s">
+        <v>96</v>
+      </c>
+      <c r="K47" t="s">
+        <v>39</v>
+      </c>
+      <c r="L47" t="s">
+        <v>99</v>
+      </c>
+      <c r="M47" t="s">
+        <v>98</v>
+      </c>
+      <c r="N47" t="s">
+        <v>99</v>
+      </c>
+      <c r="O47" t="s">
+        <v>98</v>
+      </c>
+      <c r="P47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>99</v>
+      </c>
+      <c r="R47" t="s">
+        <v>99</v>
+      </c>
+      <c r="S47" t="s">
+        <v>98</v>
+      </c>
+      <c r="T47" t="s">
+        <v>99</v>
+      </c>
+      <c r="U47" t="s">
+        <v>99</v>
+      </c>
+      <c r="V47" t="s">
+        <v>99</v>
+      </c>
+      <c r="W47" t="s">
+        <v>100</v>
+      </c>
+      <c r="X47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35">
+      <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" t="s">
+        <v>44</v>
+      </c>
+      <c r="H48" t="s">
+        <v>44</v>
+      </c>
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" t="s">
+        <v>96</v>
+      </c>
+      <c r="K48" t="s">
+        <v>39</v>
+      </c>
+      <c r="L48" t="s">
+        <v>99</v>
+      </c>
+      <c r="M48" t="s">
+        <v>99</v>
+      </c>
+      <c r="N48" t="s">
+        <v>99</v>
+      </c>
+      <c r="O48" t="s">
+        <v>99</v>
+      </c>
+      <c r="P48" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>99</v>
+      </c>
+      <c r="R48" t="s">
+        <v>99</v>
+      </c>
+      <c r="S48" t="s">
+        <v>99</v>
+      </c>
+      <c r="T48" t="s">
+        <v>44</v>
+      </c>
+      <c r="U48" t="s">
+        <v>44</v>
+      </c>
+      <c r="V48" t="s">
+        <v>44</v>
+      </c>
+      <c r="W48" t="s">
+        <v>44</v>
+      </c>
+      <c r="X48" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2441,26 +4213,103 @@
       <formula>OR($A$9="tier 3.1", $A$9="tier 4")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N22:O23 V22:W23 AG22">
+  <conditionalFormatting sqref="N15:O16 V15:W16 AG15">
     <cfRule type="expression" dxfId="0" priority="25">
-      <formula>OR($AG$22="1.1", $AG$22="1.2")</formula>
+      <formula>OR($AG$15="1.1", $AG$15="1.2")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="26">
-      <formula>OR($AG$22="2.1",$AG$22="2.2", $AG$22="2.3", $AG$22="2.4")</formula>
+      <formula>OR($AG$15="2.1",$AG$15="2.2", $AG$15="2.3", $AG$15="2.4")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="27">
-      <formula>$AG$22&gt;="3"</formula>
+      <formula>$AG$15&gt;="3"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26:O27 V26:W27 AG26">
+  <conditionalFormatting sqref="N19:O20 V19:W20 AG19">
     <cfRule type="expression" dxfId="0" priority="28">
-      <formula>OR($AG$26="1.1", $AG$26="1.2")</formula>
+      <formula>OR($AG$19="1.1", $AG$19="1.2")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="29">
-      <formula>OR($AG$26="2.1",$AG$26="2.2", $AG$26="2.3", $AG$26="2.4")</formula>
+      <formula>OR($AG$19="2.1",$AG$19="2.2", $AG$19="2.3", $AG$19="2.4")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="30">
-      <formula>$AG$26&gt;="3"</formula>
+      <formula>$AG$19&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N23:O24 V23:W24 AG23">
+    <cfRule type="expression" dxfId="0" priority="31">
+      <formula>OR($AG$23="1.1", $AG$23="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="32">
+      <formula>OR($AG$23="2.1",$AG$23="2.2", $AG$23="2.3", $AG$23="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="33">
+      <formula>$AG$23&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N27:O28 V27:W28 AG27">
+    <cfRule type="expression" dxfId="0" priority="34">
+      <formula>OR($AG$27="1.1", $AG$27="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="35">
+      <formula>OR($AG$27="2.1",$AG$27="2.2", $AG$27="2.3", $AG$27="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="36">
+      <formula>$AG$27&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N31:O32 V31:W32 AG31">
+    <cfRule type="expression" dxfId="0" priority="37">
+      <formula>OR($AG$31="1.1", $AG$31="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="38">
+      <formula>OR($AG$31="2.1",$AG$31="2.2", $AG$31="2.3", $AG$31="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="39">
+      <formula>$AG$31&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N35:O36 V35:W36 AG35">
+    <cfRule type="expression" dxfId="0" priority="40">
+      <formula>OR($AG$35="1.1", $AG$35="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="41">
+      <formula>OR($AG$35="2.1",$AG$35="2.2", $AG$35="2.3", $AG$35="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="42">
+      <formula>$AG$35&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N39:O40 V39:W40 AG39">
+    <cfRule type="expression" dxfId="0" priority="43">
+      <formula>OR($AG$39="1.1", $AG$39="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="44">
+      <formula>OR($AG$39="2.1",$AG$39="2.2", $AG$39="2.3", $AG$39="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="45">
+      <formula>$AG$39&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N43:O44 V43:W44 AG43">
+    <cfRule type="expression" dxfId="0" priority="46">
+      <formula>OR($AG$43="1.1", $AG$43="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="47">
+      <formula>OR($AG$43="2.1",$AG$43="2.2", $AG$43="2.3", $AG$43="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="48">
+      <formula>$AG$43&gt;="3"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N47:O48 V47:W48 AG47">
+    <cfRule type="expression" dxfId="0" priority="49">
+      <formula>OR($AG$47="1.1", $AG$47="1.2")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="50">
+      <formula>OR($AG$47="2.1",$AG$47="2.2", $AG$47="2.3", $AG$47="2.4")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="51">
+      <formula>$AG$47&gt;="3"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>